<commit_message>
updated Results table and metadata
</commit_message>
<xml_diff>
--- a/ResultsTable_metadata.xlsx
+++ b/ResultsTable_metadata.xlsx
@@ -282,12 +282,6 @@
     </r>
   </si>
   <si>
-    <t>HostUse combined into 2 levels: two levels: 1) Specialists (including a) monophagous species feeding only on a single host plant species, b) oligophagous species feeding on a limited number (two to four) of host plant species, and c) species that feed on lichen or fungi), and 2) Generalist (polyphagous species feeding on several (&gt; 5) host plants)</t>
-  </si>
-  <si>
-    <t>Voltinism combined into two levels: 1) Semi-and univoltine species and 2) Multivoltine species (including facultative bivoltine species)</t>
-  </si>
-  <si>
     <t>Pvalue_PopulationTrend</t>
   </si>
   <si>
@@ -295,6 +289,12 @@
   </si>
   <si>
     <t>Hypothesiswise_Response</t>
+  </si>
+  <si>
+    <t>Voltinism combined into a categorical variable two levels: 1) Semi-and univoltine species and 2) Multivoltine species (including facultative bivoltine species)</t>
+  </si>
+  <si>
+    <t>HostUse combined into a categorical variable with two levels: 1) Specialists= including monophagous species feeding only on a single host plant species,  oligophagous species feeding on a limited number (two to four) of host plant species, and species that feed on lichen or fungi, and 2) Generalist= polyphagous species feeding on several (&gt; 5) host plants.</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,7 +737,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
@@ -844,7 +844,7 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -852,7 +852,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>